<commit_message>
Tuesday Goals. I was having problems on a couple of variables, I am modelling on them.
Please change the hardcoded path from
"C:/Users/Ayush...../data/......"
to
"data/......"
</commit_message>
<xml_diff>
--- a/data/CO/2017-2018/Discipline by Gender 2017-18 Corrected.xlsx
+++ b/data/CO/2017-2018/Discipline by Gender 2017-18 Corrected.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishikth\Downloads\ds 5110 dataset\additional\2017-2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Documents\GitHub\DS-5110-Group-Project\data\CO\2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E787C2B-95BD-478A-A605-3B66F3683AD4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12940" windowHeight="4020"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12945" windowHeight="4020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$2:$Q$325</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1506,7 +1507,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1899,7 +1900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1909,15 +1910,15 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="17" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="17" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>177</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -2024,7 +2025,7 @@
       </c>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2078,7 +2079,7 @@
       </c>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2132,7 +2133,7 @@
       </c>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2186,7 +2187,7 @@
       </c>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -2240,7 +2241,7 @@
       </c>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -2294,7 +2295,7 @@
       </c>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -2348,7 +2349,7 @@
       </c>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>182</v>
       </c>
@@ -2402,7 +2403,7 @@
       </c>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -2456,7 +2457,7 @@
       </c>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>182</v>
       </c>
@@ -2510,7 +2511,7 @@
       </c>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -2564,7 +2565,7 @@
       </c>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2618,7 +2619,7 @@
       </c>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -2672,7 +2673,7 @@
       </c>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>182</v>
       </c>
@@ -2726,7 +2727,7 @@
       </c>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>182</v>
       </c>
@@ -2780,7 +2781,7 @@
       </c>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -2834,7 +2835,7 @@
       </c>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>182</v>
       </c>
@@ -2888,7 +2889,7 @@
       </c>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -2942,7 +2943,7 @@
       </c>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -2996,7 +2997,7 @@
       </c>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>182</v>
       </c>
@@ -3050,7 +3051,7 @@
       </c>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3104,7 +3105,7 @@
       </c>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -3158,7 +3159,7 @@
       </c>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -3212,7 +3213,7 @@
       </c>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -3266,7 +3267,7 @@
       </c>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>182</v>
       </c>
@@ -3320,7 +3321,7 @@
       </c>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>182</v>
       </c>
@@ -3374,7 +3375,7 @@
       </c>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>182</v>
       </c>
@@ -3428,7 +3429,7 @@
       </c>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -3482,7 +3483,7 @@
       </c>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>182</v>
       </c>
@@ -3536,7 +3537,7 @@
       </c>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -3590,7 +3591,7 @@
       </c>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -3644,7 +3645,7 @@
       </c>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -3698,7 +3699,7 @@
       </c>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>182</v>
       </c>
@@ -3752,7 +3753,7 @@
       </c>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -3806,7 +3807,7 @@
       </c>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>182</v>
       </c>
@@ -3860,7 +3861,7 @@
       </c>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -3914,7 +3915,7 @@
       </c>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>182</v>
       </c>
@@ -3968,7 +3969,7 @@
       </c>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>182</v>
       </c>
@@ -4022,7 +4023,7 @@
       </c>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>182</v>
       </c>
@@ -4076,7 +4077,7 @@
       </c>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>182</v>
       </c>
@@ -4130,7 +4131,7 @@
       </c>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>182</v>
       </c>
@@ -4184,7 +4185,7 @@
       </c>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>182</v>
       </c>
@@ -4238,7 +4239,7 @@
       </c>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>182</v>
       </c>
@@ -4292,7 +4293,7 @@
       </c>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -4346,7 +4347,7 @@
       </c>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>182</v>
       </c>
@@ -4400,7 +4401,7 @@
       </c>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>182</v>
       </c>
@@ -4454,7 +4455,7 @@
       </c>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -4508,7 +4509,7 @@
       </c>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>182</v>
       </c>
@@ -4562,7 +4563,7 @@
       </c>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -4616,7 +4617,7 @@
       </c>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -4670,7 +4671,7 @@
       </c>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>182</v>
       </c>
@@ -4724,7 +4725,7 @@
       </c>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>182</v>
       </c>
@@ -4778,7 +4779,7 @@
       </c>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>182</v>
       </c>
@@ -4832,7 +4833,7 @@
       </c>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>182</v>
       </c>
@@ -4886,7 +4887,7 @@
       </c>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>182</v>
       </c>
@@ -4940,7 +4941,7 @@
       </c>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>182</v>
       </c>
@@ -4994,7 +4995,7 @@
       </c>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -5048,7 +5049,7 @@
       </c>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -5102,7 +5103,7 @@
       </c>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -5156,7 +5157,7 @@
       </c>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -5210,7 +5211,7 @@
       </c>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>182</v>
       </c>
@@ -5264,7 +5265,7 @@
       </c>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>182</v>
       </c>
@@ -5318,7 +5319,7 @@
       </c>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>182</v>
       </c>
@@ -5372,7 +5373,7 @@
       </c>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -5426,7 +5427,7 @@
       </c>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>182</v>
       </c>
@@ -5480,7 +5481,7 @@
       </c>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>182</v>
       </c>
@@ -5534,7 +5535,7 @@
       </c>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>182</v>
       </c>
@@ -5588,7 +5589,7 @@
       </c>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -5642,7 +5643,7 @@
       </c>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>182</v>
       </c>
@@ -5696,7 +5697,7 @@
       </c>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>182</v>
       </c>
@@ -5750,7 +5751,7 @@
       </c>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -5804,7 +5805,7 @@
       </c>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>182</v>
       </c>
@@ -5858,7 +5859,7 @@
       </c>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>182</v>
       </c>
@@ -5912,7 +5913,7 @@
       </c>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -5966,7 +5967,7 @@
       </c>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>182</v>
       </c>
@@ -6020,7 +6021,7 @@
       </c>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>182</v>
       </c>
@@ -6074,7 +6075,7 @@
       </c>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>182</v>
       </c>
@@ -6128,7 +6129,7 @@
       </c>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>182</v>
       </c>
@@ -6182,7 +6183,7 @@
       </c>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>182</v>
       </c>
@@ -6236,7 +6237,7 @@
       </c>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>182</v>
       </c>
@@ -6290,7 +6291,7 @@
       </c>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -6344,7 +6345,7 @@
       </c>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>182</v>
       </c>
@@ -6398,7 +6399,7 @@
       </c>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>182</v>
       </c>
@@ -6452,7 +6453,7 @@
       </c>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>182</v>
       </c>
@@ -6506,7 +6507,7 @@
       </c>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>182</v>
       </c>
@@ -6560,7 +6561,7 @@
       </c>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>182</v>
       </c>
@@ -6614,7 +6615,7 @@
       </c>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>182</v>
       </c>
@@ -6668,7 +6669,7 @@
       </c>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>182</v>
       </c>
@@ -6722,7 +6723,7 @@
       </c>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>182</v>
       </c>
@@ -6776,7 +6777,7 @@
       </c>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>182</v>
       </c>
@@ -6830,7 +6831,7 @@
       </c>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>182</v>
       </c>
@@ -6884,7 +6885,7 @@
       </c>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -6938,7 +6939,7 @@
       </c>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>182</v>
       </c>
@@ -6992,7 +6993,7 @@
       </c>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>182</v>
       </c>
@@ -7046,7 +7047,7 @@
       </c>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>182</v>
       </c>
@@ -7100,7 +7101,7 @@
       </c>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>182</v>
       </c>
@@ -7154,7 +7155,7 @@
       </c>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>182</v>
       </c>
@@ -7208,7 +7209,7 @@
       </c>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>182</v>
       </c>
@@ -7262,7 +7263,7 @@
       </c>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>182</v>
       </c>
@@ -7316,7 +7317,7 @@
       </c>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>182</v>
       </c>
@@ -7370,7 +7371,7 @@
       </c>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>182</v>
       </c>
@@ -7424,7 +7425,7 @@
       </c>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>182</v>
       </c>
@@ -7478,7 +7479,7 @@
       </c>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>182</v>
       </c>
@@ -7532,7 +7533,7 @@
       </c>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>182</v>
       </c>
@@ -7586,7 +7587,7 @@
       </c>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>182</v>
       </c>
@@ -7640,7 +7641,7 @@
       </c>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>182</v>
       </c>
@@ -7694,7 +7695,7 @@
       </c>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>182</v>
       </c>
@@ -7748,7 +7749,7 @@
       </c>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>182</v>
       </c>
@@ -7802,7 +7803,7 @@
       </c>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>182</v>
       </c>
@@ -7856,7 +7857,7 @@
       </c>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>182</v>
       </c>
@@ -7910,7 +7911,7 @@
       </c>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>182</v>
       </c>
@@ -7964,7 +7965,7 @@
       </c>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>182</v>
       </c>
@@ -8018,7 +8019,7 @@
       </c>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>182</v>
       </c>
@@ -8072,7 +8073,7 @@
       </c>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>182</v>
       </c>
@@ -8126,7 +8127,7 @@
       </c>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>182</v>
       </c>
@@ -8180,7 +8181,7 @@
       </c>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>182</v>
       </c>
@@ -8234,7 +8235,7 @@
       </c>
       <c r="R117" s="4"/>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>182</v>
       </c>
@@ -8288,7 +8289,7 @@
       </c>
       <c r="R118" s="4"/>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>182</v>
       </c>
@@ -8342,7 +8343,7 @@
       </c>
       <c r="R119" s="4"/>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>182</v>
       </c>
@@ -8396,7 +8397,7 @@
       </c>
       <c r="R120" s="4"/>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>182</v>
       </c>
@@ -8450,7 +8451,7 @@
       </c>
       <c r="R121" s="4"/>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>182</v>
       </c>
@@ -8504,7 +8505,7 @@
       </c>
       <c r="R122" s="4"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>182</v>
       </c>
@@ -8558,7 +8559,7 @@
       </c>
       <c r="R123" s="4"/>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>182</v>
       </c>
@@ -8612,7 +8613,7 @@
       </c>
       <c r="R124" s="4"/>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>182</v>
       </c>
@@ -8666,7 +8667,7 @@
       </c>
       <c r="R125" s="4"/>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>182</v>
       </c>
@@ -8720,7 +8721,7 @@
       </c>
       <c r="R126" s="4"/>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>182</v>
       </c>
@@ -8774,7 +8775,7 @@
       </c>
       <c r="R127" s="4"/>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>182</v>
       </c>
@@ -8828,7 +8829,7 @@
       </c>
       <c r="R128" s="4"/>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>182</v>
       </c>
@@ -8882,7 +8883,7 @@
       </c>
       <c r="R129" s="4"/>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>182</v>
       </c>
@@ -8936,7 +8937,7 @@
       </c>
       <c r="R130" s="4"/>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>182</v>
       </c>
@@ -8990,7 +8991,7 @@
       </c>
       <c r="R131" s="4"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>182</v>
       </c>
@@ -9044,7 +9045,7 @@
       </c>
       <c r="R132" s="4"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>182</v>
       </c>
@@ -9098,7 +9099,7 @@
       </c>
       <c r="R133" s="4"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>182</v>
       </c>
@@ -9152,7 +9153,7 @@
       </c>
       <c r="R134" s="4"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>182</v>
       </c>
@@ -9206,7 +9207,7 @@
       </c>
       <c r="R135" s="4"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>182</v>
       </c>
@@ -9260,7 +9261,7 @@
       </c>
       <c r="R136" s="4"/>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>182</v>
       </c>
@@ -9314,7 +9315,7 @@
       </c>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>182</v>
       </c>
@@ -9368,7 +9369,7 @@
       </c>
       <c r="R138" s="4"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>182</v>
       </c>
@@ -9422,7 +9423,7 @@
       </c>
       <c r="R139" s="4"/>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>182</v>
       </c>
@@ -9476,7 +9477,7 @@
       </c>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>182</v>
       </c>
@@ -9530,7 +9531,7 @@
       </c>
       <c r="R141" s="4"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>182</v>
       </c>
@@ -9584,7 +9585,7 @@
       </c>
       <c r="R142" s="4"/>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>182</v>
       </c>
@@ -9638,7 +9639,7 @@
       </c>
       <c r="R143" s="4"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>182</v>
       </c>
@@ -9692,7 +9693,7 @@
       </c>
       <c r="R144" s="4"/>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>182</v>
       </c>
@@ -9746,7 +9747,7 @@
       </c>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>182</v>
       </c>
@@ -9800,7 +9801,7 @@
       </c>
       <c r="R146" s="4"/>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>182</v>
       </c>
@@ -9854,7 +9855,7 @@
       </c>
       <c r="R147" s="4"/>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>182</v>
       </c>
@@ -9908,7 +9909,7 @@
       </c>
       <c r="R148" s="4"/>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>182</v>
       </c>
@@ -9962,7 +9963,7 @@
       </c>
       <c r="R149" s="4"/>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>182</v>
       </c>
@@ -10016,7 +10017,7 @@
       </c>
       <c r="R150" s="4"/>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>182</v>
       </c>
@@ -10070,7 +10071,7 @@
       </c>
       <c r="R151" s="4"/>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>182</v>
       </c>
@@ -10124,7 +10125,7 @@
       </c>
       <c r="R152" s="4"/>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>182</v>
       </c>
@@ -10178,7 +10179,7 @@
       </c>
       <c r="R153" s="4"/>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>182</v>
       </c>
@@ -10232,7 +10233,7 @@
       </c>
       <c r="R154" s="4"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>182</v>
       </c>
@@ -10286,7 +10287,7 @@
       </c>
       <c r="R155" s="4"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>182</v>
       </c>
@@ -10340,7 +10341,7 @@
       </c>
       <c r="R156" s="4"/>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>182</v>
       </c>
@@ -10394,7 +10395,7 @@
       </c>
       <c r="R157" s="4"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>182</v>
       </c>
@@ -10448,7 +10449,7 @@
       </c>
       <c r="R158" s="4"/>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>182</v>
       </c>
@@ -10502,7 +10503,7 @@
       </c>
       <c r="R159" s="4"/>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>182</v>
       </c>
@@ -10556,7 +10557,7 @@
       </c>
       <c r="R160" s="4"/>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>182</v>
       </c>
@@ -10610,7 +10611,7 @@
       </c>
       <c r="R161" s="4"/>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>182</v>
       </c>
@@ -10664,7 +10665,7 @@
       </c>
       <c r="R162" s="4"/>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>182</v>
       </c>
@@ -10718,7 +10719,7 @@
       </c>
       <c r="R163" s="4"/>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>182</v>
       </c>
@@ -10772,7 +10773,7 @@
       </c>
       <c r="R164" s="4"/>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>182</v>
       </c>
@@ -10826,7 +10827,7 @@
       </c>
       <c r="R165" s="4"/>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>182</v>
       </c>
@@ -10880,7 +10881,7 @@
       </c>
       <c r="R166" s="4"/>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>182</v>
       </c>
@@ -10934,7 +10935,7 @@
       </c>
       <c r="R167" s="4"/>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>182</v>
       </c>
@@ -10988,7 +10989,7 @@
       </c>
       <c r="R168" s="4"/>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>182</v>
       </c>
@@ -11042,7 +11043,7 @@
       </c>
       <c r="R169" s="4"/>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>182</v>
       </c>
@@ -11096,7 +11097,7 @@
       </c>
       <c r="R170" s="4"/>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>182</v>
       </c>
@@ -11150,7 +11151,7 @@
       </c>
       <c r="R171" s="4"/>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>182</v>
       </c>
@@ -11204,7 +11205,7 @@
       </c>
       <c r="R172" s="4"/>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>182</v>
       </c>
@@ -11258,7 +11259,7 @@
       </c>
       <c r="R173" s="4"/>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>182</v>
       </c>
@@ -11312,7 +11313,7 @@
       </c>
       <c r="R174" s="4"/>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -11366,7 +11367,7 @@
       </c>
       <c r="R175" s="4"/>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>182</v>
       </c>
@@ -11420,7 +11421,7 @@
       </c>
       <c r="R176" s="4"/>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>182</v>
       </c>
@@ -11474,7 +11475,7 @@
       </c>
       <c r="R177" s="4"/>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>182</v>
       </c>
@@ -11528,7 +11529,7 @@
       </c>
       <c r="R178" s="4"/>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>182</v>
       </c>
@@ -11582,7 +11583,7 @@
       </c>
       <c r="R179" s="4"/>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>182</v>
       </c>
@@ -11636,7 +11637,7 @@
       </c>
       <c r="R180" s="4"/>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -11690,7 +11691,7 @@
       </c>
       <c r="R181" s="4"/>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -11744,7 +11745,7 @@
       </c>
       <c r="R182" s="4"/>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -11798,7 +11799,7 @@
       </c>
       <c r="R183" s="4"/>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -11852,7 +11853,7 @@
       </c>
       <c r="R184" s="4"/>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>182</v>
       </c>
@@ -11906,7 +11907,7 @@
       </c>
       <c r="R185" s="4"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>182</v>
       </c>
@@ -11960,7 +11961,7 @@
       </c>
       <c r="R186" s="4"/>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>182</v>
       </c>
@@ -12014,7 +12015,7 @@
       </c>
       <c r="R187" s="4"/>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>182</v>
       </c>
@@ -12068,7 +12069,7 @@
       </c>
       <c r="R188" s="4"/>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>182</v>
       </c>
@@ -12122,7 +12123,7 @@
       </c>
       <c r="R189" s="4"/>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>182</v>
       </c>
@@ -12176,7 +12177,7 @@
       </c>
       <c r="R190" s="4"/>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>182</v>
       </c>
@@ -12230,7 +12231,7 @@
       </c>
       <c r="R191" s="4"/>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>182</v>
       </c>
@@ -12284,7 +12285,7 @@
       </c>
       <c r="R192" s="4"/>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>182</v>
       </c>
@@ -12338,7 +12339,7 @@
       </c>
       <c r="R193" s="4"/>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>182</v>
       </c>
@@ -12392,7 +12393,7 @@
       </c>
       <c r="R194" s="4"/>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>182</v>
       </c>
@@ -12446,7 +12447,7 @@
       </c>
       <c r="R195" s="4"/>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>182</v>
       </c>
@@ -12500,7 +12501,7 @@
       </c>
       <c r="R196" s="4"/>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>182</v>
       </c>
@@ -12554,7 +12555,7 @@
       </c>
       <c r="R197" s="4"/>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>182</v>
       </c>
@@ -12608,7 +12609,7 @@
       </c>
       <c r="R198" s="4"/>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>182</v>
       </c>
@@ -12662,7 +12663,7 @@
       </c>
       <c r="R199" s="4"/>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>182</v>
       </c>
@@ -12716,7 +12717,7 @@
       </c>
       <c r="R200" s="4"/>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>182</v>
       </c>
@@ -12770,7 +12771,7 @@
       </c>
       <c r="R201" s="4"/>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>182</v>
       </c>
@@ -12824,7 +12825,7 @@
       </c>
       <c r="R202" s="4"/>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>182</v>
       </c>
@@ -12878,7 +12879,7 @@
       </c>
       <c r="R203" s="4"/>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>182</v>
       </c>
@@ -12932,7 +12933,7 @@
       </c>
       <c r="R204" s="4"/>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>182</v>
       </c>
@@ -12986,7 +12987,7 @@
       </c>
       <c r="R205" s="4"/>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>182</v>
       </c>
@@ -13040,7 +13041,7 @@
       </c>
       <c r="R206" s="4"/>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>182</v>
       </c>
@@ -13094,7 +13095,7 @@
       </c>
       <c r="R207" s="4"/>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>182</v>
       </c>
@@ -13148,7 +13149,7 @@
       </c>
       <c r="R208" s="4"/>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>182</v>
       </c>
@@ -13202,7 +13203,7 @@
       </c>
       <c r="R209" s="4"/>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>182</v>
       </c>
@@ -13256,7 +13257,7 @@
       </c>
       <c r="R210" s="4"/>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>182</v>
       </c>
@@ -13310,7 +13311,7 @@
       </c>
       <c r="R211" s="4"/>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>182</v>
       </c>
@@ -13364,7 +13365,7 @@
       </c>
       <c r="R212" s="4"/>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>182</v>
       </c>
@@ -13418,7 +13419,7 @@
       </c>
       <c r="R213" s="4"/>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>182</v>
       </c>
@@ -13472,7 +13473,7 @@
       </c>
       <c r="R214" s="4"/>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>182</v>
       </c>
@@ -13526,7 +13527,7 @@
       </c>
       <c r="R215" s="4"/>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>182</v>
       </c>
@@ -13580,7 +13581,7 @@
       </c>
       <c r="R216" s="4"/>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>182</v>
       </c>
@@ -13634,7 +13635,7 @@
       </c>
       <c r="R217" s="4"/>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>182</v>
       </c>
@@ -13688,7 +13689,7 @@
       </c>
       <c r="R218" s="4"/>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>182</v>
       </c>
@@ -13742,7 +13743,7 @@
       </c>
       <c r="R219" s="4"/>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>182</v>
       </c>
@@ -13796,7 +13797,7 @@
       </c>
       <c r="R220" s="4"/>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>182</v>
       </c>
@@ -13850,7 +13851,7 @@
       </c>
       <c r="R221" s="4"/>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>182</v>
       </c>
@@ -13904,7 +13905,7 @@
       </c>
       <c r="R222" s="4"/>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>182</v>
       </c>
@@ -13958,7 +13959,7 @@
       </c>
       <c r="R223" s="4"/>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>182</v>
       </c>
@@ -14012,7 +14013,7 @@
       </c>
       <c r="R224" s="4"/>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>182</v>
       </c>
@@ -14066,7 +14067,7 @@
       </c>
       <c r="R225" s="4"/>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>182</v>
       </c>
@@ -14120,7 +14121,7 @@
       </c>
       <c r="R226" s="4"/>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>182</v>
       </c>
@@ -14174,7 +14175,7 @@
       </c>
       <c r="R227" s="4"/>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>182</v>
       </c>
@@ -14228,7 +14229,7 @@
       </c>
       <c r="R228" s="4"/>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>182</v>
       </c>
@@ -14282,7 +14283,7 @@
       </c>
       <c r="R229" s="4"/>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>182</v>
       </c>
@@ -14336,7 +14337,7 @@
       </c>
       <c r="R230" s="4"/>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>182</v>
       </c>
@@ -14390,7 +14391,7 @@
       </c>
       <c r="R231" s="4"/>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>182</v>
       </c>
@@ -14444,7 +14445,7 @@
       </c>
       <c r="R232" s="4"/>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>182</v>
       </c>
@@ -14498,7 +14499,7 @@
       </c>
       <c r="R233" s="4"/>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>182</v>
       </c>
@@ -14552,7 +14553,7 @@
       </c>
       <c r="R234" s="4"/>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>182</v>
       </c>
@@ -14606,7 +14607,7 @@
       </c>
       <c r="R235" s="4"/>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>182</v>
       </c>
@@ -14660,7 +14661,7 @@
       </c>
       <c r="R236" s="4"/>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>182</v>
       </c>
@@ -14714,7 +14715,7 @@
       </c>
       <c r="R237" s="4"/>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>182</v>
       </c>
@@ -14768,7 +14769,7 @@
       </c>
       <c r="R238" s="4"/>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>182</v>
       </c>
@@ -14822,7 +14823,7 @@
       </c>
       <c r="R239" s="4"/>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>182</v>
       </c>
@@ -14876,7 +14877,7 @@
       </c>
       <c r="R240" s="4"/>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>182</v>
       </c>
@@ -14930,7 +14931,7 @@
       </c>
       <c r="R241" s="4"/>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>182</v>
       </c>
@@ -14984,7 +14985,7 @@
       </c>
       <c r="R242" s="4"/>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>182</v>
       </c>
@@ -15038,7 +15039,7 @@
       </c>
       <c r="R243" s="4"/>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>182</v>
       </c>
@@ -15092,7 +15093,7 @@
       </c>
       <c r="R244" s="4"/>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>182</v>
       </c>
@@ -15146,7 +15147,7 @@
       </c>
       <c r="R245" s="4"/>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>182</v>
       </c>
@@ -15200,7 +15201,7 @@
       </c>
       <c r="R246" s="4"/>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>182</v>
       </c>
@@ -15254,7 +15255,7 @@
       </c>
       <c r="R247" s="4"/>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>182</v>
       </c>
@@ -15308,7 +15309,7 @@
       </c>
       <c r="R248" s="4"/>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>182</v>
       </c>
@@ -15362,7 +15363,7 @@
       </c>
       <c r="R249" s="4"/>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>182</v>
       </c>
@@ -15416,7 +15417,7 @@
       </c>
       <c r="R250" s="4"/>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>182</v>
       </c>
@@ -15470,7 +15471,7 @@
       </c>
       <c r="R251" s="4"/>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>182</v>
       </c>
@@ -15524,7 +15525,7 @@
       </c>
       <c r="R252" s="4"/>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>182</v>
       </c>
@@ -15578,7 +15579,7 @@
       </c>
       <c r="R253" s="4"/>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>182</v>
       </c>
@@ -15632,7 +15633,7 @@
       </c>
       <c r="R254" s="4"/>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>182</v>
       </c>
@@ -15686,7 +15687,7 @@
       </c>
       <c r="R255" s="4"/>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>182</v>
       </c>
@@ -15740,7 +15741,7 @@
       </c>
       <c r="R256" s="4"/>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>182</v>
       </c>
@@ -15794,7 +15795,7 @@
       </c>
       <c r="R257" s="4"/>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>182</v>
       </c>
@@ -15848,7 +15849,7 @@
       </c>
       <c r="R258" s="4"/>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>182</v>
       </c>
@@ -15902,7 +15903,7 @@
       </c>
       <c r="R259" s="4"/>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>182</v>
       </c>
@@ -15956,7 +15957,7 @@
       </c>
       <c r="R260" s="4"/>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>182</v>
       </c>
@@ -16010,7 +16011,7 @@
       </c>
       <c r="R261" s="4"/>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>182</v>
       </c>
@@ -16064,7 +16065,7 @@
       </c>
       <c r="R262" s="4"/>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>182</v>
       </c>
@@ -16118,7 +16119,7 @@
       </c>
       <c r="R263" s="4"/>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>182</v>
       </c>
@@ -16172,7 +16173,7 @@
       </c>
       <c r="R264" s="4"/>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>182</v>
       </c>
@@ -16226,7 +16227,7 @@
       </c>
       <c r="R265" s="4"/>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>182</v>
       </c>
@@ -16280,7 +16281,7 @@
       </c>
       <c r="R266" s="4"/>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>182</v>
       </c>
@@ -16334,7 +16335,7 @@
       </c>
       <c r="R267" s="4"/>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>182</v>
       </c>
@@ -16388,7 +16389,7 @@
       </c>
       <c r="R268" s="4"/>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>182</v>
       </c>
@@ -16442,7 +16443,7 @@
       </c>
       <c r="R269" s="4"/>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>182</v>
       </c>
@@ -16496,7 +16497,7 @@
       </c>
       <c r="R270" s="4"/>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>182</v>
       </c>
@@ -16550,7 +16551,7 @@
       </c>
       <c r="R271" s="4"/>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>182</v>
       </c>
@@ -16604,7 +16605,7 @@
       </c>
       <c r="R272" s="4"/>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>182</v>
       </c>
@@ -16658,7 +16659,7 @@
       </c>
       <c r="R273" s="4"/>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>182</v>
       </c>
@@ -16712,7 +16713,7 @@
       </c>
       <c r="R274" s="4"/>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>182</v>
       </c>
@@ -16766,7 +16767,7 @@
       </c>
       <c r="R275" s="4"/>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>182</v>
       </c>
@@ -16820,7 +16821,7 @@
       </c>
       <c r="R276" s="4"/>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>182</v>
       </c>
@@ -16874,7 +16875,7 @@
       </c>
       <c r="R277" s="4"/>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>182</v>
       </c>
@@ -16928,7 +16929,7 @@
       </c>
       <c r="R278" s="4"/>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>182</v>
       </c>
@@ -16982,7 +16983,7 @@
       </c>
       <c r="R279" s="4"/>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>182</v>
       </c>
@@ -17036,7 +17037,7 @@
       </c>
       <c r="R280" s="4"/>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>182</v>
       </c>
@@ -17090,7 +17091,7 @@
       </c>
       <c r="R281" s="4"/>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>182</v>
       </c>
@@ -17144,7 +17145,7 @@
       </c>
       <c r="R282" s="4"/>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>182</v>
       </c>
@@ -17198,7 +17199,7 @@
       </c>
       <c r="R283" s="4"/>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>182</v>
       </c>
@@ -17252,7 +17253,7 @@
       </c>
       <c r="R284" s="4"/>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>182</v>
       </c>
@@ -17306,7 +17307,7 @@
       </c>
       <c r="R285" s="4"/>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>182</v>
       </c>
@@ -17360,7 +17361,7 @@
       </c>
       <c r="R286" s="4"/>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>182</v>
       </c>
@@ -17414,7 +17415,7 @@
       </c>
       <c r="R287" s="4"/>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>182</v>
       </c>
@@ -17468,7 +17469,7 @@
       </c>
       <c r="R288" s="4"/>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>182</v>
       </c>
@@ -17522,7 +17523,7 @@
       </c>
       <c r="R289" s="4"/>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>182</v>
       </c>
@@ -17576,7 +17577,7 @@
       </c>
       <c r="R290" s="4"/>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>182</v>
       </c>
@@ -17630,7 +17631,7 @@
       </c>
       <c r="R291" s="4"/>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>182</v>
       </c>
@@ -17684,7 +17685,7 @@
       </c>
       <c r="R292" s="4"/>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>182</v>
       </c>
@@ -17738,7 +17739,7 @@
       </c>
       <c r="R293" s="4"/>
     </row>
-    <row r="294" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>182</v>
       </c>
@@ -17792,7 +17793,7 @@
       </c>
       <c r="R294" s="4"/>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>182</v>
       </c>
@@ -17846,7 +17847,7 @@
       </c>
       <c r="R295" s="4"/>
     </row>
-    <row r="296" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>182</v>
       </c>
@@ -17900,7 +17901,7 @@
       </c>
       <c r="R296" s="4"/>
     </row>
-    <row r="297" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>182</v>
       </c>
@@ -17954,7 +17955,7 @@
       </c>
       <c r="R297" s="4"/>
     </row>
-    <row r="298" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>182</v>
       </c>
@@ -18008,7 +18009,7 @@
       </c>
       <c r="R298" s="4"/>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>182</v>
       </c>
@@ -18062,7 +18063,7 @@
       </c>
       <c r="R299" s="4"/>
     </row>
-    <row r="300" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>182</v>
       </c>
@@ -18116,7 +18117,7 @@
       </c>
       <c r="R300" s="4"/>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>182</v>
       </c>
@@ -18170,7 +18171,7 @@
       </c>
       <c r="R301" s="4"/>
     </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>182</v>
       </c>
@@ -18224,7 +18225,7 @@
       </c>
       <c r="R302" s="4"/>
     </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>182</v>
       </c>
@@ -18278,7 +18279,7 @@
       </c>
       <c r="R303" s="4"/>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>182</v>
       </c>
@@ -18332,7 +18333,7 @@
       </c>
       <c r="R304" s="4"/>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>182</v>
       </c>
@@ -18386,7 +18387,7 @@
       </c>
       <c r="R305" s="4"/>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>182</v>
       </c>
@@ -18440,7 +18441,7 @@
       </c>
       <c r="R306" s="4"/>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>182</v>
       </c>
@@ -18494,7 +18495,7 @@
       </c>
       <c r="R307" s="4"/>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>182</v>
       </c>
@@ -18548,7 +18549,7 @@
       </c>
       <c r="R308" s="4"/>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>182</v>
       </c>
@@ -18602,7 +18603,7 @@
       </c>
       <c r="R309" s="4"/>
     </row>
-    <row r="310" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>182</v>
       </c>
@@ -18656,7 +18657,7 @@
       </c>
       <c r="R310" s="4"/>
     </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>182</v>
       </c>
@@ -18710,7 +18711,7 @@
       </c>
       <c r="R311" s="4"/>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>182</v>
       </c>
@@ -18764,7 +18765,7 @@
       </c>
       <c r="R312" s="4"/>
     </row>
-    <row r="313" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>182</v>
       </c>
@@ -18818,7 +18819,7 @@
       </c>
       <c r="R313" s="4"/>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>182</v>
       </c>
@@ -18872,7 +18873,7 @@
       </c>
       <c r="R314" s="4"/>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>182</v>
       </c>
@@ -18926,7 +18927,7 @@
       </c>
       <c r="R315" s="4"/>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>182</v>
       </c>
@@ -18980,7 +18981,7 @@
       </c>
       <c r="R316" s="4"/>
     </row>
-    <row r="317" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>182</v>
       </c>
@@ -19034,7 +19035,7 @@
       </c>
       <c r="R317" s="4"/>
     </row>
-    <row r="318" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>182</v>
       </c>
@@ -19088,7 +19089,7 @@
       </c>
       <c r="R318" s="4"/>
     </row>
-    <row r="319" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>182</v>
       </c>
@@ -19142,7 +19143,7 @@
       </c>
       <c r="R319" s="4"/>
     </row>
-    <row r="320" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>182</v>
       </c>
@@ -19196,7 +19197,7 @@
       </c>
       <c r="R320" s="4"/>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>182</v>
       </c>
@@ -19250,7 +19251,7 @@
       </c>
       <c r="R321" s="4"/>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>182</v>
       </c>
@@ -19304,7 +19305,7 @@
       </c>
       <c r="R322" s="4"/>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>182</v>
       </c>
@@ -19358,7 +19359,7 @@
       </c>
       <c r="R323" s="4"/>
     </row>
-    <row r="324" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>182</v>
       </c>
@@ -19412,7 +19413,7 @@
       </c>
       <c r="R324" s="4"/>
     </row>
-    <row r="325" spans="1:18" s="10" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:18" s="10" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>483</v>
       </c>

</xml_diff>